<commit_message>
Update send email Minerva
</commit_message>
<xml_diff>
--- a/TestCase Automation - Minerva.xlsx
+++ b/TestCase Automation - Minerva.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="370">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="372">
   <si>
     <t>ID TestScenario</t>
   </si>
@@ -1133,6 +1133,12 @@
   </si>
   <si>
     <t>07/14/2020 10:50:13</t>
+  </si>
+  <si>
+    <t>07/15/2020 22:29:15</t>
+  </si>
+  <si>
+    <t>07/15/2020 22:31:36</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1185,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="504">
+  <fills count="568">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3696,6 +3702,326 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill>
+        <fgColor indexed="40"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="40"/>
       </patternFill>
     </fill>
   </fills>
@@ -3751,7 +4077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="293">
+  <cellXfs count="325">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4067,6 +4393,38 @@
     <xf numFmtId="0" fontId="0" fillId="499" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="501" borderId="0" xfId="0" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="503" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="505" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="507" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="509" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="511" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="513" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="515" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="517" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="519" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="521" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="523" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="525" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="527" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="529" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="531" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="533" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="535" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="537" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="539" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="541" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="543" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="545" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="547" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="549" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="551" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="553" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="555" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="557" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="559" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="561" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="563" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="565" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="567" borderId="0" xfId="0" applyFill="true"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5209,7 +5567,7 @@
       <c r="G3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="270" t="s">
+      <c r="H3" s="302" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5233,7 +5591,7 @@
         <v>110</v>
       </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="271" t="s">
+      <c r="H4" s="303" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5257,7 +5615,7 @@
         <v>58</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="272" t="s">
+      <c r="H5" s="304" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5281,7 +5639,7 @@
         <v>14</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="273" t="s">
+      <c r="H6" s="305" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5305,7 +5663,7 @@
         <v>58</v>
       </c>
       <c r="G7" s="7"/>
-      <c r="H7" s="274" t="s">
+      <c r="H7" s="306" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5329,7 +5687,7 @@
         <v>14</v>
       </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="275" t="s">
+      <c r="H8" s="307" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5353,7 +5711,7 @@
         <v>58</v>
       </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="276" t="s">
+      <c r="H9" s="308" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5379,7 +5737,7 @@
       <c r="G10" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="H10" s="277" t="s">
+      <c r="H10" s="309" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5399,7 +5757,7 @@
         <v>37</v>
       </c>
       <c r="G11" s="7"/>
-      <c r="H11" s="278" t="s">
+      <c r="H11" s="310" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5423,7 +5781,7 @@
         <v>318</v>
       </c>
       <c r="G12" s="7"/>
-      <c r="H12" t="s" s="279">
+      <c r="H12" t="s" s="311">
         <v>118</v>
       </c>
     </row>
@@ -5449,7 +5807,7 @@
       <c r="G13" s="7" t="s">
         <v>341</v>
       </c>
-      <c r="H13" s="280" t="s">
+      <c r="H13" s="312" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5469,7 +5827,7 @@
         <v>37</v>
       </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="281" t="s">
+      <c r="H14" s="313" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5495,7 +5853,7 @@
       <c r="G15" s="7" t="s">
         <v>342</v>
       </c>
-      <c r="H15" s="282" t="s">
+      <c r="H15" s="314" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5515,7 +5873,7 @@
         <v>37</v>
       </c>
       <c r="G16" s="7"/>
-      <c r="H16" s="283" t="s">
+      <c r="H16" s="315" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5541,7 +5899,7 @@
       <c r="G17" s="7" t="s">
         <v>344</v>
       </c>
-      <c r="H17" s="284" t="s">
+      <c r="H17" s="316" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5561,7 +5919,7 @@
         <v>37</v>
       </c>
       <c r="G18" s="7"/>
-      <c r="H18" s="285" t="s">
+      <c r="H18" s="317" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5587,7 +5945,7 @@
       <c r="G19" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="H19" s="286" t="s">
+      <c r="H19" s="318" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5607,7 +5965,7 @@
         <v>37</v>
       </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="287" t="s">
+      <c r="H20" s="319" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5631,7 +5989,7 @@
         <v>14</v>
       </c>
       <c r="G21" s="7"/>
-      <c r="H21" s="288" t="s">
+      <c r="H21" s="320" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5655,7 +6013,7 @@
         <v>58</v>
       </c>
       <c r="G22" s="7"/>
-      <c r="H22" s="289" t="s">
+      <c r="H22" s="321" t="s">
         <v>118</v>
       </c>
     </row>
@@ -5675,8 +6033,8 @@
         <v>351</v>
       </c>
       <c r="G23" s="7"/>
-      <c r="H23" s="290" t="s">
-        <v>362</v>
+      <c r="H23" s="322" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -5749,14 +6107,14 @@
       <c r="C2" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="291" t="s">
-        <v>362</v>
+      <c r="D2" s="323" t="s">
+        <v>118</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="F2" s="292" t="s">
-        <v>369</v>
+      <c r="F2" s="324" t="s">
+        <v>371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>